<commit_message>
added SO2 photolysis to SpO2 and SOpO
</commit_message>
<xml_diff>
--- a/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
+++ b/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01a63ffdd6170d0a/Desktop/copy REU Research/bluejay/Venus-Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C41CBD6-16E1-4A09-B17C-ADC8B0CE5F7F}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C145249B-6BFE-4F88-9C7F-059F918BA490}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="552" windowWidth="21528" windowHeight="11832" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="552" windowWidth="21528" windowHeight="11832" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8863" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8893" uniqueCount="479">
   <si>
     <t>R1</t>
   </si>
@@ -1501,7 +1501,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1526,6 +1526,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1539,7 +1545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1549,6 +1555,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1865,7 +1872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y304"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E282" sqref="E282"/>
     </sheetView>
@@ -63780,11 +63787,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -64938,6 +64945,58 @@
       </c>
       <c r="K37" s="4" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B38" t="s">
+        <v>444</v>
+      </c>
+      <c r="C38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>256</v>
+      </c>
+      <c r="E38" t="s">
+        <v>475</v>
+      </c>
+      <c r="F38" t="s">
+        <v>291</v>
+      </c>
+      <c r="G38" t="s">
+        <v>291</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B39" t="s">
+        <v>443</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>256</v>
+      </c>
+      <c r="E39" t="s">
+        <v>475</v>
+      </c>
+      <c r="F39" t="s">
+        <v>291</v>
+      </c>
+      <c r="G39" t="s">
+        <v>291</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -66072,11 +66131,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Y92"/>
+  <dimension ref="A1:Y96"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56:XFD59"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93:XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -69794,7 +69853,7 @@
       <c r="A92" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C92" t="s">
@@ -69817,6 +69876,68 @@
       </c>
       <c r="K92" s="4" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B93" t="s">
+        <v>444</v>
+      </c>
+      <c r="C93" t="s">
+        <v>31</v>
+      </c>
+      <c r="D93" t="s">
+        <v>256</v>
+      </c>
+      <c r="E93" t="s">
+        <v>475</v>
+      </c>
+      <c r="F93" t="s">
+        <v>291</v>
+      </c>
+      <c r="G93" t="s">
+        <v>291</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B94" t="s">
+        <v>443</v>
+      </c>
+      <c r="C94" t="s">
+        <v>69</v>
+      </c>
+      <c r="D94" t="s">
+        <v>256</v>
+      </c>
+      <c r="E94" t="s">
+        <v>475</v>
+      </c>
+      <c r="F94" t="s">
+        <v>291</v>
+      </c>
+      <c r="G94" t="s">
+        <v>291</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made HDpCltoHClpDorDClpH mass scaleing
</commit_message>
<xml_diff>
--- a/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
+++ b/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01a63ffdd6170d0a/Desktop/copy REU Research/bluejay/Venus-Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94D3D621-BFC0-4D2B-B7EE-353EFA6FB0F7}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5072E0A-A865-46C2-BD4F-868AE022A8D7}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="900" windowWidth="21528" windowHeight="11832" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="900" windowWidth="21528" windowHeight="11832" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ion reactions" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9435" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9449" uniqueCount="545">
   <si>
     <t>R1</t>
   </si>
@@ -46701,11 +46701,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y326"/>
+  <dimension ref="A1:Y327"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A281" sqref="A281:XFD281"/>
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F289" sqref="F289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -63111,6 +63111,7 @@
       <c r="B288" s="10" t="s">
         <v>416</v>
       </c>
+      <c r="C288" s="12"/>
       <c r="D288" t="s">
         <v>478</v>
       </c>
@@ -63120,14 +63121,20 @@
       <c r="G288">
         <v>2</v>
       </c>
+      <c r="H288">
+        <v>3</v>
+      </c>
+      <c r="I288">
+        <v>2</v>
+      </c>
       <c r="L288" s="1">
-        <v>1.1000000000000001E-11</v>
+        <v>3.9000000000000001E-11</v>
       </c>
       <c r="M288">
         <v>0</v>
       </c>
-      <c r="N288">
-        <v>-1130</v>
+      <c r="N288" s="1">
+        <v>-2310</v>
       </c>
       <c r="O288">
         <v>0</v>
@@ -63151,13 +63158,10 @@
         <v>0</v>
       </c>
       <c r="V288" t="s">
-        <v>522</v>
-      </c>
-      <c r="W288" t="s">
-        <v>523</v>
-      </c>
-      <c r="X288" s="4" t="s">
-        <v>479</v>
+        <v>423</v>
+      </c>
+      <c r="W288" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="Y288" t="s">
         <v>418</v>
@@ -63165,34 +63169,35 @@
     </row>
     <row r="289" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B289" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="B289" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="C289" s="12"/>
       <c r="D289" t="s">
-        <v>478</v>
+        <v>415</v>
       </c>
       <c r="E289" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G289">
         <v>2</v>
       </c>
       <c r="H289">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="I289">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="L289" s="1">
-        <v>1.7999999999999999E-11</v>
+        <v>3.9000000000000001E-11</v>
       </c>
       <c r="M289">
         <v>0</v>
       </c>
       <c r="N289" s="1">
-        <v>169</v>
+        <v>-2310</v>
       </c>
       <c r="O289">
         <v>0</v>
@@ -63216,9 +63221,9 @@
         <v>0</v>
       </c>
       <c r="V289" t="s">
-        <v>427</v>
-      </c>
-      <c r="W289" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="W289" s="3" t="s">
         <v>87</v>
       </c>
       <c r="Y289" t="s">
@@ -63227,58 +63232,58 @@
     </row>
     <row r="290" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
-        <v>72</v>
+        <v>416</v>
       </c>
       <c r="B290" s="6" t="s">
-        <v>424</v>
+        <v>83</v>
       </c>
       <c r="D290" t="s">
         <v>478</v>
       </c>
       <c r="E290" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="G290">
         <v>2</v>
       </c>
       <c r="H290">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="I290">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="L290" s="1">
-        <v>9.9999999999999998E-13</v>
+        <v>1.7999999999999999E-11</v>
       </c>
       <c r="M290">
         <v>0</v>
       </c>
       <c r="N290" s="1">
-        <v>-4800</v>
+        <v>169</v>
       </c>
       <c r="O290">
         <v>0</v>
       </c>
-      <c r="P290" s="1">
+      <c r="P290">
         <v>0</v>
       </c>
       <c r="Q290">
         <v>0</v>
       </c>
-      <c r="R290" s="1">
+      <c r="R290">
         <v>0</v>
       </c>
       <c r="S290">
         <v>0</v>
       </c>
-      <c r="T290" s="1">
+      <c r="T290">
         <v>0</v>
       </c>
       <c r="U290">
         <v>0</v>
       </c>
       <c r="V290" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="W290" s="5" t="s">
         <v>87</v>
@@ -63295,10 +63300,10 @@
         <v>424</v>
       </c>
       <c r="D291" t="s">
-        <v>415</v>
+        <v>478</v>
       </c>
       <c r="E291" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="G291">
         <v>2</v>
@@ -63351,58 +63356,58 @@
     </row>
     <row r="292" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B292" s="6" t="s">
         <v>424</v>
       </c>
       <c r="D292" t="s">
-        <v>83</v>
+        <v>415</v>
       </c>
       <c r="E292" t="s">
-        <v>416</v>
-      </c>
-      <c r="G292" s="8">
+        <v>80</v>
+      </c>
+      <c r="G292">
         <v>2</v>
       </c>
       <c r="H292">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I292">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="L292" s="1">
-        <v>1.7999999999999999E-11</v>
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="M292">
         <v>0</v>
       </c>
       <c r="N292" s="1">
-        <v>169</v>
+        <v>-4800</v>
       </c>
       <c r="O292">
         <v>0</v>
       </c>
-      <c r="P292">
+      <c r="P292" s="1">
         <v>0</v>
       </c>
       <c r="Q292">
         <v>0</v>
       </c>
-      <c r="R292">
+      <c r="R292" s="1">
         <v>0</v>
       </c>
       <c r="S292">
         <v>0</v>
       </c>
-      <c r="T292">
+      <c r="T292" s="1">
         <v>0</v>
       </c>
       <c r="U292">
         <v>0</v>
       </c>
       <c r="V292" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="W292" s="5" t="s">
         <v>87</v>
@@ -63415,26 +63420,32 @@
       <c r="A293" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B293" s="10" t="s">
+      <c r="B293" s="6" t="s">
         <v>424</v>
       </c>
       <c r="D293" t="s">
-        <v>478</v>
+        <v>83</v>
       </c>
       <c r="E293" t="s">
-        <v>69</v>
-      </c>
-      <c r="G293">
+        <v>416</v>
+      </c>
+      <c r="G293" s="8">
         <v>2</v>
       </c>
+      <c r="H293">
+        <v>18</v>
+      </c>
+      <c r="I293">
+        <v>17</v>
+      </c>
       <c r="L293" s="1">
-        <v>1.6900000000000001E-13</v>
+        <v>1.7999999999999999E-11</v>
       </c>
       <c r="M293">
         <v>0</v>
       </c>
-      <c r="N293">
-        <v>363</v>
+      <c r="N293" s="1">
+        <v>169</v>
       </c>
       <c r="O293">
         <v>0</v>
@@ -63458,10 +63469,10 @@
         <v>0</v>
       </c>
       <c r="V293" t="s">
-        <v>480</v>
-      </c>
-      <c r="W293" t="s">
-        <v>482</v>
+        <v>427</v>
+      </c>
+      <c r="W293" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="Y293" t="s">
         <v>418</v>
@@ -63469,35 +63480,28 @@
     </row>
     <row r="294" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B294" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="C294" s="12"/>
+        <v>424</v>
+      </c>
       <c r="D294" t="s">
-        <v>72</v>
+        <v>478</v>
       </c>
       <c r="E294" t="s">
-        <v>416</v>
+        <v>69</v>
       </c>
       <c r="G294">
         <v>2</v>
       </c>
-      <c r="H294">
-        <v>2</v>
-      </c>
-      <c r="I294">
-        <v>1</v>
-      </c>
       <c r="L294" s="1">
-        <v>1.4900000000000002E-11</v>
+        <v>1.6900000000000001E-13</v>
       </c>
       <c r="M294">
         <v>0</v>
       </c>
-      <c r="N294" s="1">
-        <v>-1760</v>
+      <c r="N294">
+        <v>363</v>
       </c>
       <c r="O294">
         <v>0</v>
@@ -63521,10 +63525,10 @@
         <v>0</v>
       </c>
       <c r="V294" t="s">
-        <v>420</v>
-      </c>
-      <c r="W294" s="5" t="s">
-        <v>87</v>
+        <v>480</v>
+      </c>
+      <c r="W294" t="s">
+        <v>482</v>
       </c>
       <c r="Y294" t="s">
         <v>418</v>
@@ -63532,33 +63536,40 @@
     </row>
     <row r="295" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
-        <v>478</v>
+        <v>71</v>
       </c>
       <c r="B295" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="C295" s="12"/>
       <c r="D295" t="s">
-        <v>415</v>
+        <v>72</v>
       </c>
       <c r="E295" t="s">
-        <v>71</v>
+        <v>416</v>
       </c>
       <c r="G295">
         <v>2</v>
       </c>
+      <c r="H295">
+        <v>2</v>
+      </c>
+      <c r="I295">
+        <v>1</v>
+      </c>
       <c r="L295" s="1">
-        <v>1.4399999999999999E-10</v>
+        <v>1.4900000000000002E-11</v>
       </c>
       <c r="M295">
         <v>0</v>
       </c>
       <c r="N295" s="1">
-        <v>-481</v>
+        <v>-1760</v>
       </c>
       <c r="O295">
         <v>0</v>
       </c>
-      <c r="P295" s="1">
+      <c r="P295">
         <v>0</v>
       </c>
       <c r="Q295">
@@ -63577,13 +63588,10 @@
         <v>0</v>
       </c>
       <c r="V295" t="s">
-        <v>522</v>
-      </c>
-      <c r="W295" t="s">
-        <v>501</v>
-      </c>
-      <c r="X295" s="4" t="s">
-        <v>479</v>
+        <v>420</v>
+      </c>
+      <c r="W295" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="Y295" t="s">
         <v>418</v>
@@ -63597,22 +63605,22 @@
         <v>33</v>
       </c>
       <c r="D296" t="s">
-        <v>72</v>
+        <v>415</v>
       </c>
       <c r="E296" t="s">
-        <v>416</v>
+        <v>71</v>
       </c>
       <c r="G296">
         <v>2</v>
       </c>
       <c r="L296" s="1">
-        <v>1.3E-11</v>
+        <v>1.4399999999999999E-10</v>
       </c>
       <c r="M296">
         <v>0</v>
       </c>
       <c r="N296" s="1">
-        <v>-1575</v>
+        <v>-481</v>
       </c>
       <c r="O296">
         <v>0</v>
@@ -63636,10 +63644,10 @@
         <v>0</v>
       </c>
       <c r="V296" t="s">
-        <v>500</v>
+        <v>522</v>
       </c>
       <c r="W296" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="X296" s="4" t="s">
         <v>479</v>
@@ -63653,10 +63661,10 @@
         <v>478</v>
       </c>
       <c r="B297" s="10" t="s">
-        <v>416</v>
+        <v>33</v>
       </c>
       <c r="D297" t="s">
-        <v>478</v>
+        <v>72</v>
       </c>
       <c r="E297" t="s">
         <v>416</v>
@@ -63665,13 +63673,13 @@
         <v>2</v>
       </c>
       <c r="L297" s="1">
-        <v>2.5400000000000001E-12</v>
+        <v>1.3E-11</v>
       </c>
       <c r="M297">
         <v>0</v>
       </c>
       <c r="N297" s="1">
-        <v>-3180</v>
+        <v>-1575</v>
       </c>
       <c r="O297">
         <v>0</v>
@@ -63695,10 +63703,13 @@
         <v>0</v>
       </c>
       <c r="V297" t="s">
-        <v>406</v>
+        <v>500</v>
       </c>
       <c r="W297" t="s">
-        <v>483</v>
+        <v>499</v>
+      </c>
+      <c r="X297" s="4" t="s">
+        <v>479</v>
       </c>
       <c r="Y297" t="s">
         <v>418</v>
@@ -63709,10 +63720,10 @@
         <v>478</v>
       </c>
       <c r="B298" s="10" t="s">
-        <v>31</v>
+        <v>416</v>
       </c>
       <c r="D298" t="s">
-        <v>80</v>
+        <v>478</v>
       </c>
       <c r="E298" t="s">
         <v>416</v>
@@ -63721,18 +63732,18 @@
         <v>2</v>
       </c>
       <c r="L298" s="1">
-        <v>3.7E-12</v>
+        <v>2.5400000000000001E-12</v>
       </c>
       <c r="M298">
         <v>0</v>
       </c>
       <c r="N298" s="1">
-        <v>-3520</v>
+        <v>-3180</v>
       </c>
       <c r="O298">
         <v>0</v>
       </c>
-      <c r="P298">
+      <c r="P298" s="1">
         <v>0</v>
       </c>
       <c r="Q298">
@@ -63751,10 +63762,10 @@
         <v>0</v>
       </c>
       <c r="V298" t="s">
-        <v>487</v>
+        <v>406</v>
       </c>
       <c r="W298" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="Y298" t="s">
         <v>418</v>
@@ -63765,30 +63776,30 @@
         <v>478</v>
       </c>
       <c r="B299" s="10" t="s">
-        <v>485</v>
+        <v>31</v>
       </c>
       <c r="D299" t="s">
-        <v>424</v>
+        <v>80</v>
       </c>
       <c r="E299" t="s">
-        <v>71</v>
+        <v>416</v>
       </c>
       <c r="G299">
         <v>2</v>
       </c>
       <c r="L299" s="1">
-        <v>6E-11</v>
+        <v>3.7E-12</v>
       </c>
       <c r="M299">
         <v>0</v>
       </c>
       <c r="N299" s="1">
-        <v>0</v>
+        <v>-3520</v>
       </c>
       <c r="O299">
         <v>0</v>
       </c>
-      <c r="P299" s="1">
+      <c r="P299">
         <v>0</v>
       </c>
       <c r="Q299">
@@ -63806,14 +63817,11 @@
       <c r="U299">
         <v>0</v>
       </c>
-      <c r="V299">
-        <v>298</v>
+      <c r="V299" t="s">
+        <v>487</v>
       </c>
       <c r="W299" t="s">
-        <v>488</v>
-      </c>
-      <c r="X299" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="Y299" t="s">
         <v>418</v>
@@ -63827,16 +63835,16 @@
         <v>485</v>
       </c>
       <c r="D300" t="s">
-        <v>80</v>
+        <v>424</v>
       </c>
       <c r="E300" t="s">
-        <v>416</v>
+        <v>71</v>
       </c>
       <c r="G300">
         <v>2</v>
       </c>
       <c r="L300" s="1">
-        <v>1.06E-10</v>
+        <v>6E-11</v>
       </c>
       <c r="M300">
         <v>0</v>
@@ -63870,6 +63878,9 @@
       </c>
       <c r="W300" t="s">
         <v>488</v>
+      </c>
+      <c r="X300" s="4" t="s">
+        <v>489</v>
       </c>
       <c r="Y300" t="s">
         <v>418</v>
@@ -63880,10 +63891,10 @@
         <v>478</v>
       </c>
       <c r="B301" s="10" t="s">
-        <v>52</v>
+        <v>485</v>
       </c>
       <c r="D301" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E301" t="s">
         <v>416</v>
@@ -63892,18 +63903,18 @@
         <v>2</v>
       </c>
       <c r="L301" s="1">
-        <v>4.2800000000000003E-12</v>
+        <v>1.06E-10</v>
       </c>
       <c r="M301">
         <v>0</v>
       </c>
-      <c r="N301">
-        <v>-767</v>
+      <c r="N301" s="1">
+        <v>0</v>
       </c>
       <c r="O301">
         <v>0</v>
       </c>
-      <c r="P301">
+      <c r="P301" s="1">
         <v>0</v>
       </c>
       <c r="Q301">
@@ -63921,11 +63932,11 @@
       <c r="U301">
         <v>0</v>
       </c>
-      <c r="V301" t="s">
-        <v>525</v>
-      </c>
-      <c r="W301" s="3" t="s">
-        <v>526</v>
+      <c r="V301">
+        <v>298</v>
+      </c>
+      <c r="W301" t="s">
+        <v>488</v>
       </c>
       <c r="Y301" t="s">
         <v>418</v>
@@ -63933,10 +63944,10 @@
     </row>
     <row r="302" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
-        <v>415</v>
+        <v>478</v>
       </c>
       <c r="B302" s="10" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D302" t="s">
         <v>76</v>
@@ -63947,20 +63958,19 @@
       <c r="G302">
         <v>2</v>
       </c>
-      <c r="K302" s="1"/>
       <c r="L302" s="1">
-        <v>8.1249999999999995E-18</v>
+        <v>4.2800000000000003E-12</v>
       </c>
       <c r="M302">
-        <v>1.85</v>
-      </c>
-      <c r="N302" s="1">
-        <v>300</v>
+        <v>0</v>
+      </c>
+      <c r="N302">
+        <v>-767</v>
       </c>
       <c r="O302">
         <v>0</v>
       </c>
-      <c r="P302" s="1">
+      <c r="P302">
         <v>0</v>
       </c>
       <c r="Q302">
@@ -63979,10 +63989,10 @@
         <v>0</v>
       </c>
       <c r="V302" t="s">
-        <v>176</v>
+        <v>525</v>
       </c>
       <c r="W302" s="3" t="s">
-        <v>490</v>
+        <v>526</v>
       </c>
       <c r="Y302" t="s">
         <v>418</v>
@@ -63990,25 +64000,29 @@
     </row>
     <row r="303" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
-        <v>454</v>
+        <v>415</v>
       </c>
       <c r="B303" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D303" t="s">
-        <v>459</v>
+        <v>76</v>
+      </c>
+      <c r="E303" t="s">
+        <v>416</v>
       </c>
       <c r="G303">
         <v>2</v>
       </c>
+      <c r="K303" s="1"/>
       <c r="L303" s="1">
-        <v>1.2E-15</v>
+        <v>8.1249999999999995E-18</v>
       </c>
       <c r="M303">
-        <v>0</v>
-      </c>
-      <c r="N303">
-        <v>0</v>
+        <v>1.85</v>
+      </c>
+      <c r="N303" s="1">
+        <v>300</v>
       </c>
       <c r="O303">
         <v>0</v>
@@ -64031,11 +64045,11 @@
       <c r="U303">
         <v>0</v>
       </c>
-      <c r="V303">
-        <v>298</v>
-      </c>
-      <c r="W303" s="5" t="s">
-        <v>461</v>
+      <c r="V303" t="s">
+        <v>176</v>
+      </c>
+      <c r="W303" s="3" t="s">
+        <v>490</v>
       </c>
       <c r="Y303" t="s">
         <v>418</v>
@@ -64046,23 +64060,14 @@
         <v>454</v>
       </c>
       <c r="B304" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D304" t="s">
-        <v>542</v>
+        <v>459</v>
       </c>
       <c r="G304">
         <v>2</v>
       </c>
-      <c r="H304">
-        <v>19</v>
-      </c>
-      <c r="I304">
-        <v>18</v>
-      </c>
-      <c r="J304">
-        <v>-0.5</v>
-      </c>
       <c r="L304" s="1">
         <v>1.2E-15</v>
       </c>
@@ -64097,30 +64102,36 @@
         <v>298</v>
       </c>
       <c r="W304" s="5" t="s">
-        <v>87</v>
+        <v>461</v>
       </c>
       <c r="Y304" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="305" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A305" t="s">
-        <v>52</v>
-      </c>
-      <c r="B305" t="s">
-        <v>52</v>
+      <c r="A305" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B305" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="D305" t="s">
-        <v>79</v>
-      </c>
-      <c r="E305" t="s">
-        <v>31</v>
+        <v>542</v>
       </c>
       <c r="G305">
         <v>2</v>
       </c>
-      <c r="L305">
-        <v>1.8E-12</v>
+      <c r="H305">
+        <v>19</v>
+      </c>
+      <c r="I305">
+        <v>18</v>
+      </c>
+      <c r="J305">
+        <v>-0.5</v>
+      </c>
+      <c r="L305" s="1">
+        <v>1.2E-15</v>
       </c>
       <c r="M305">
         <v>0</v>
@@ -64131,7 +64142,7 @@
       <c r="O305">
         <v>0</v>
       </c>
-      <c r="P305">
+      <c r="P305" s="1">
         <v>0</v>
       </c>
       <c r="Q305">
@@ -64149,43 +64160,46 @@
       <c r="U305">
         <v>0</v>
       </c>
-      <c r="V305" t="s">
-        <v>229</v>
-      </c>
-      <c r="W305" t="s">
-        <v>105</v>
+      <c r="V305">
+        <v>298</v>
+      </c>
+      <c r="W305" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="Y305" t="s">
-        <v>42</v>
+        <v>418</v>
       </c>
     </row>
     <row r="306" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B306" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D306" t="s">
-        <v>88</v>
+        <v>79</v>
+      </c>
+      <c r="E306" t="s">
+        <v>31</v>
       </c>
       <c r="G306">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L306">
-        <v>1</v>
+        <v>1.8E-12</v>
       </c>
       <c r="M306">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N306">
         <v>0</v>
       </c>
       <c r="O306">
-        <v>2E-35</v>
+        <v>0</v>
       </c>
       <c r="P306">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="Q306">
         <v>0</v>
@@ -64203,10 +64217,10 @@
         <v>0</v>
       </c>
       <c r="V306" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="W306" t="s">
-        <v>231</v>
+        <v>105</v>
       </c>
       <c r="Y306" t="s">
         <v>42</v>
@@ -64217,10 +64231,10 @@
         <v>47</v>
       </c>
       <c r="B307" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D307" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="G307">
         <v>4</v>
@@ -64259,7 +64273,7 @@
         <v>230</v>
       </c>
       <c r="W307" t="s">
-        <v>49</v>
+        <v>231</v>
       </c>
       <c r="Y307" t="s">
         <v>42</v>
@@ -64270,10 +64284,10 @@
         <v>47</v>
       </c>
       <c r="B308" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D308" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G308">
         <v>4</v>
@@ -64282,19 +64296,19 @@
         <v>1</v>
       </c>
       <c r="M308">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N308">
-        <v>-1509</v>
+        <v>0</v>
       </c>
       <c r="O308">
-        <v>1.7E-33</v>
+        <v>2E-35</v>
       </c>
       <c r="P308">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="Q308">
-        <v>-1509</v>
+        <v>0</v>
       </c>
       <c r="R308">
         <v>0</v>
@@ -64306,13 +64320,13 @@
         <v>0</v>
       </c>
       <c r="U308">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="V308" t="s">
-        <v>57</v>
+        <v>230</v>
       </c>
       <c r="W308" t="s">
-        <v>139</v>
+        <v>49</v>
       </c>
       <c r="Y308" t="s">
         <v>42</v>
@@ -64320,13 +64334,13 @@
     </row>
     <row r="309" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B309" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D309" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G309">
         <v>4</v>
@@ -64338,16 +64352,16 @@
         <v>0</v>
       </c>
       <c r="N309">
-        <v>0</v>
+        <v>-1509</v>
       </c>
       <c r="O309">
-        <v>5.0000000000000004E-32</v>
+        <v>1.7E-33</v>
       </c>
       <c r="P309">
         <v>0</v>
       </c>
       <c r="Q309">
-        <v>0</v>
+        <v>-1509</v>
       </c>
       <c r="R309">
         <v>0</v>
@@ -64359,13 +64373,13 @@
         <v>0</v>
       </c>
       <c r="U309">
-        <v>0</v>
-      </c>
-      <c r="V309">
-        <v>298</v>
+        <v>0.4</v>
+      </c>
+      <c r="V309" t="s">
+        <v>57</v>
       </c>
       <c r="W309" t="s">
-        <v>232</v>
+        <v>139</v>
       </c>
       <c r="Y309" t="s">
         <v>42</v>
@@ -64373,34 +64387,34 @@
     </row>
     <row r="310" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B310" t="s">
         <v>33</v>
       </c>
       <c r="D310" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="G310">
         <v>4</v>
       </c>
       <c r="L310">
-        <v>2.5300000000000002E-9</v>
+        <v>1</v>
       </c>
       <c r="M310">
-        <v>-0.41</v>
+        <v>0</v>
       </c>
       <c r="N310">
         <v>0</v>
       </c>
       <c r="O310">
-        <v>9.5599999999999997E-29</v>
+        <v>5.0000000000000004E-32</v>
       </c>
       <c r="P310">
-        <v>-1.17</v>
+        <v>0</v>
       </c>
       <c r="Q310">
-        <v>-212</v>
+        <v>0</v>
       </c>
       <c r="R310">
         <v>0</v>
@@ -64412,16 +64426,13 @@
         <v>0</v>
       </c>
       <c r="U310">
-        <v>0.82</v>
-      </c>
-      <c r="V310" t="s">
-        <v>57</v>
+        <v>0</v>
+      </c>
+      <c r="V310">
+        <v>298</v>
       </c>
       <c r="W310" t="s">
-        <v>233</v>
-      </c>
-      <c r="X310" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Y310" t="s">
         <v>42</v>
@@ -64432,31 +64443,31 @@
         <v>61</v>
       </c>
       <c r="B311" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D311" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="G311">
         <v>4</v>
       </c>
       <c r="L311">
-        <v>4.8999999999999996E-10</v>
+        <v>2.5300000000000002E-9</v>
       </c>
       <c r="M311">
-        <v>-0.4</v>
+        <v>-0.41</v>
       </c>
       <c r="N311">
         <v>0</v>
       </c>
       <c r="O311">
-        <v>9.1999999999999994E-28</v>
+        <v>9.5599999999999997E-29</v>
       </c>
       <c r="P311">
-        <v>-1.6</v>
+        <v>-1.17</v>
       </c>
       <c r="Q311">
-        <v>0</v>
+        <v>-212</v>
       </c>
       <c r="R311">
         <v>0</v>
@@ -64468,13 +64479,13 @@
         <v>0</v>
       </c>
       <c r="U311">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="V311" t="s">
-        <v>235</v>
+        <v>57</v>
       </c>
       <c r="W311" t="s">
-        <v>49</v>
+        <v>233</v>
       </c>
       <c r="X311" t="s">
         <v>234</v>
@@ -64485,34 +64496,34 @@
     </row>
     <row r="312" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
+        <v>61</v>
+      </c>
+      <c r="B312" t="s">
         <v>31</v>
       </c>
-      <c r="B312" t="s">
-        <v>26</v>
-      </c>
       <c r="D312" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="G312">
         <v>4</v>
       </c>
       <c r="L312">
-        <v>1</v>
+        <v>4.8999999999999996E-10</v>
       </c>
       <c r="M312">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="N312">
         <v>0</v>
       </c>
       <c r="O312">
-        <v>5.46E-33</v>
+        <v>9.1999999999999994E-28</v>
       </c>
       <c r="P312">
-        <v>0</v>
+        <v>-1.6</v>
       </c>
       <c r="Q312">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="R312">
         <v>0</v>
@@ -64524,13 +64535,13 @@
         <v>0</v>
       </c>
       <c r="U312">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="V312" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="W312" t="s">
-        <v>237</v>
+        <v>49</v>
       </c>
       <c r="X312" t="s">
         <v>234</v>
@@ -64541,28 +64552,19 @@
     </row>
     <row r="313" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="B313" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D313" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="G313">
         <v>4</v>
       </c>
-      <c r="H313">
-        <v>18</v>
-      </c>
-      <c r="I313">
-        <v>17</v>
-      </c>
-      <c r="J313">
-        <v>-0.5</v>
-      </c>
       <c r="L313">
-        <v>2.6000000000000001E-11</v>
+        <v>1</v>
       </c>
       <c r="M313">
         <v>0</v>
@@ -64571,13 +64573,13 @@
         <v>0</v>
       </c>
       <c r="O313">
-        <v>6.6000000000000006E-29</v>
+        <v>5.46E-33</v>
       </c>
       <c r="P313">
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="Q313">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="R313">
         <v>0</v>
@@ -64589,10 +64591,16 @@
         <v>0</v>
       </c>
       <c r="U313">
-        <v>0.5</v>
+        <v>0.4</v>
+      </c>
+      <c r="V313" t="s">
+        <v>236</v>
       </c>
       <c r="W313" t="s">
-        <v>87</v>
+        <v>237</v>
+      </c>
+      <c r="X313" t="s">
+        <v>234</v>
       </c>
       <c r="Y313" t="s">
         <v>42</v>
@@ -64600,17 +64608,26 @@
     </row>
     <row r="314" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B314" t="s">
         <v>52</v>
       </c>
       <c r="D314" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G314">
         <v>4</v>
       </c>
+      <c r="H314">
+        <v>18</v>
+      </c>
+      <c r="I314">
+        <v>17</v>
+      </c>
+      <c r="J314">
+        <v>-0.5</v>
+      </c>
       <c r="L314">
         <v>2.6000000000000001E-11</v>
       </c>
@@ -64641,46 +64658,40 @@
       <c r="U314">
         <v>0.5</v>
       </c>
-      <c r="V314" t="s">
-        <v>176</v>
-      </c>
       <c r="W314" t="s">
-        <v>49</v>
-      </c>
-      <c r="X314" t="s">
-        <v>238</v>
+        <v>87</v>
       </c>
       <c r="Y314" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="315" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B315" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D315" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="G315">
         <v>4</v>
       </c>
       <c r="L315">
-        <v>1</v>
+        <v>2.6000000000000001E-11</v>
       </c>
       <c r="M315">
-        <v>-0.9</v>
+        <v>0</v>
       </c>
       <c r="N315">
         <v>0</v>
       </c>
       <c r="O315">
-        <v>4.7499999999999999E-34</v>
+        <v>6.6000000000000006E-29</v>
       </c>
       <c r="P315">
-        <v>-0.9</v>
+        <v>-0.8</v>
       </c>
       <c r="Q315">
         <v>0</v>
@@ -64695,51 +64706,48 @@
         <v>0</v>
       </c>
       <c r="U315">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="V315" t="s">
+        <v>176</v>
       </c>
       <c r="W315" t="s">
-        <v>105</v>
+        <v>49</v>
+      </c>
+      <c r="X315" t="s">
+        <v>238</v>
       </c>
       <c r="Y315" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="316" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B316" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D316" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="G316">
-        <v>5</v>
-      </c>
-      <c r="H316">
-        <v>18</v>
-      </c>
-      <c r="I316">
-        <v>17</v>
-      </c>
-      <c r="J316">
-        <v>-0.5</v>
+        <v>4</v>
       </c>
       <c r="L316">
-        <v>6.6242246742872797E-16</v>
+        <v>1</v>
       </c>
       <c r="M316">
-        <v>1.3</v>
+        <v>-0.9</v>
       </c>
       <c r="N316">
         <v>0</v>
       </c>
       <c r="O316">
-        <v>1.7330926013789299E-29</v>
+        <v>4.7499999999999999E-34</v>
       </c>
       <c r="P316">
-        <v>-1.4</v>
+        <v>-0.9</v>
       </c>
       <c r="Q316">
         <v>0</v>
@@ -64757,7 +64765,7 @@
         <v>0</v>
       </c>
       <c r="W316" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="Y316" t="s">
         <v>42</v>
@@ -64768,14 +64776,23 @@
         <v>47</v>
       </c>
       <c r="B317" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D317" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="G317">
         <v>5</v>
       </c>
+      <c r="H317">
+        <v>18</v>
+      </c>
+      <c r="I317">
+        <v>17</v>
+      </c>
+      <c r="J317">
+        <v>-0.5</v>
+      </c>
       <c r="L317">
         <v>6.6242246742872797E-16</v>
       </c>
@@ -64807,7 +64824,7 @@
         <v>0</v>
       </c>
       <c r="W317" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="Y317" t="s">
         <v>42</v>
@@ -64815,40 +64832,31 @@
     </row>
     <row r="318" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B318" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D318" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="G318">
         <v>5</v>
       </c>
-      <c r="H318">
-        <v>2</v>
-      </c>
-      <c r="I318">
-        <v>1</v>
-      </c>
-      <c r="J318">
-        <v>-0.5</v>
-      </c>
       <c r="L318">
-        <v>2.39682878878546E-11</v>
+        <v>6.6242246742872797E-16</v>
       </c>
       <c r="M318">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="N318">
         <v>0</v>
       </c>
       <c r="O318">
-        <v>1.46130309220551E-28</v>
+        <v>1.7330926013789299E-29</v>
       </c>
       <c r="P318">
-        <v>-1.3</v>
+        <v>-1.4</v>
       </c>
       <c r="Q318">
         <v>0</v>
@@ -64866,7 +64874,7 @@
         <v>0</v>
       </c>
       <c r="W318" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="Y318" t="s">
         <v>42</v>
@@ -64874,19 +64882,28 @@
     </row>
     <row r="319" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B319" t="s">
         <v>69</v>
       </c>
       <c r="D319" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G319">
         <v>5</v>
       </c>
+      <c r="H319">
+        <v>2</v>
+      </c>
+      <c r="I319">
+        <v>1</v>
+      </c>
+      <c r="J319">
+        <v>-0.5</v>
+      </c>
       <c r="L319">
-        <v>2.39683E-11</v>
+        <v>2.39682878878546E-11</v>
       </c>
       <c r="M319">
         <v>0.2</v>
@@ -64895,7 +64912,7 @@
         <v>0</v>
       </c>
       <c r="O319">
-        <v>1.4613E-28</v>
+        <v>1.46130309220551E-28</v>
       </c>
       <c r="P319">
         <v>-1.3</v>
@@ -64916,7 +64933,7 @@
         <v>0</v>
       </c>
       <c r="W319" t="s">
-        <v>224</v>
+        <v>87</v>
       </c>
       <c r="Y319" t="s">
         <v>42</v>
@@ -64924,31 +64941,31 @@
     </row>
     <row r="320" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B320" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D320" t="s">
-        <v>239</v>
+        <v>81</v>
       </c>
       <c r="G320">
         <v>5</v>
       </c>
       <c r="L320">
-        <v>6.3699999999999997E-11</v>
+        <v>2.39683E-11</v>
       </c>
       <c r="M320">
-        <v>-0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N320">
         <v>0</v>
       </c>
       <c r="O320">
-        <v>1.93E-24</v>
+        <v>1.4613E-28</v>
       </c>
       <c r="P320">
-        <v>-2.6</v>
+        <v>-1.3</v>
       </c>
       <c r="Q320">
         <v>0</v>
@@ -64966,7 +64983,7 @@
         <v>0</v>
       </c>
       <c r="W320" t="s">
-        <v>105</v>
+        <v>224</v>
       </c>
       <c r="Y320" t="s">
         <v>42</v>
@@ -64974,31 +64991,31 @@
     </row>
     <row r="321" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B321" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="D321" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G321">
         <v>5</v>
       </c>
       <c r="L321">
-        <v>2.21E-11</v>
+        <v>6.3699999999999997E-11</v>
       </c>
       <c r="M321">
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="N321">
         <v>0</v>
       </c>
       <c r="O321">
-        <v>5.0199999999999997E-23</v>
+        <v>1.93E-24</v>
       </c>
       <c r="P321">
-        <v>-3.4</v>
+        <v>-2.6</v>
       </c>
       <c r="Q321">
         <v>0</v>
@@ -65027,28 +65044,28 @@
         <v>91</v>
       </c>
       <c r="B322" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="D322" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="G322">
         <v>5</v>
       </c>
       <c r="L322">
-        <v>1.19E-9</v>
+        <v>2.21E-11</v>
       </c>
       <c r="M322">
-        <v>-0.7</v>
+        <v>-0.3</v>
       </c>
       <c r="N322">
         <v>0</v>
       </c>
       <c r="O322">
-        <v>7.1899999999999994E-27</v>
+        <v>5.0199999999999997E-23</v>
       </c>
       <c r="P322">
-        <v>-1.8</v>
+        <v>-3.4</v>
       </c>
       <c r="Q322">
         <v>0</v>
@@ -65077,28 +65094,28 @@
         <v>91</v>
       </c>
       <c r="B323" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D323" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="G323">
         <v>5</v>
       </c>
       <c r="L323">
-        <v>2.8E-11</v>
+        <v>1.19E-9</v>
       </c>
       <c r="M323">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
       <c r="N323">
         <v>0</v>
       </c>
       <c r="O323">
-        <v>4.8600000000000002E-23</v>
+        <v>7.1899999999999994E-27</v>
       </c>
       <c r="P323">
-        <v>-3</v>
+        <v>-1.8</v>
       </c>
       <c r="Q323">
         <v>0</v>
@@ -65130,25 +65147,25 @@
         <v>52</v>
       </c>
       <c r="D324" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G324">
         <v>5</v>
       </c>
       <c r="L324">
-        <v>7270000000000</v>
+        <v>2.8E-11</v>
       </c>
       <c r="M324">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="N324">
         <v>0</v>
       </c>
       <c r="O324">
-        <v>4.1700000000000001E-22</v>
+        <v>4.8600000000000002E-23</v>
       </c>
       <c r="P324">
-        <v>-3.9</v>
+        <v>-3</v>
       </c>
       <c r="Q324">
         <v>0</v>
@@ -65174,43 +65191,31 @@
     </row>
     <row r="325" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="B325" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D325" t="s">
-        <v>63</v>
-      </c>
-      <c r="E325" t="s">
-        <v>71</v>
+        <v>242</v>
       </c>
       <c r="G325">
-        <v>6</v>
-      </c>
-      <c r="H325">
-        <v>18</v>
-      </c>
-      <c r="I325">
-        <v>17</v>
-      </c>
-      <c r="J325">
+        <v>5</v>
+      </c>
+      <c r="L325">
+        <v>7270000000000</v>
+      </c>
+      <c r="M325">
         <v>-0.5</v>
       </c>
-      <c r="L325">
-        <v>1.62846954489706E-6</v>
-      </c>
-      <c r="M325">
-        <v>6.1</v>
-      </c>
       <c r="N325">
         <v>0</v>
       </c>
       <c r="O325">
-        <v>4.8957418118048899E-15</v>
+        <v>4.1700000000000001E-22</v>
       </c>
       <c r="P325">
-        <v>0.6</v>
+        <v>-3.9</v>
       </c>
       <c r="Q325">
         <v>0</v>
@@ -65228,7 +65233,7 @@
         <v>0</v>
       </c>
       <c r="W325" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="Y325" t="s">
         <v>42</v>
@@ -65239,17 +65244,26 @@
         <v>47</v>
       </c>
       <c r="B326" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D326" t="s">
         <v>63</v>
       </c>
       <c r="E326" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="G326">
         <v>6</v>
       </c>
+      <c r="H326">
+        <v>18</v>
+      </c>
+      <c r="I326">
+        <v>17</v>
+      </c>
+      <c r="J326">
+        <v>-0.5</v>
+      </c>
       <c r="L326">
         <v>1.62846954489706E-6</v>
       </c>
@@ -65281,9 +65295,62 @@
         <v>0</v>
       </c>
       <c r="W326" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y326" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="327" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>47</v>
+      </c>
+      <c r="B327" t="s">
+        <v>52</v>
+      </c>
+      <c r="D327" t="s">
+        <v>63</v>
+      </c>
+      <c r="E327" t="s">
+        <v>33</v>
+      </c>
+      <c r="G327">
+        <v>6</v>
+      </c>
+      <c r="L327">
+        <v>1.62846954489706E-6</v>
+      </c>
+      <c r="M327">
+        <v>6.1</v>
+      </c>
+      <c r="N327">
+        <v>0</v>
+      </c>
+      <c r="O327">
+        <v>4.8957418118048899E-15</v>
+      </c>
+      <c r="P327">
+        <v>0.6</v>
+      </c>
+      <c r="Q327">
+        <v>0</v>
+      </c>
+      <c r="R327">
+        <v>0</v>
+      </c>
+      <c r="S327">
+        <v>0</v>
+      </c>
+      <c r="T327">
+        <v>0</v>
+      </c>
+      <c r="U327">
+        <v>0</v>
+      </c>
+      <c r="W327" t="s">
         <v>224</v>
       </c>
-      <c r="Y326" t="s">
+      <c r="Y327" t="s">
         <v>42</v>
       </c>
     </row>
@@ -67767,11 +67834,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Y175"/>
+  <dimension ref="A1:Y177"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A175" sqref="A175:XFD175"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -73804,6 +73871,65 @@
         <v>513</v>
       </c>
       <c r="Y175" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="177" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A177" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B177" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="D177" t="s">
+        <v>478</v>
+      </c>
+      <c r="E177" t="s">
+        <v>33</v>
+      </c>
+      <c r="G177">
+        <v>2</v>
+      </c>
+      <c r="L177" s="1">
+        <v>1.1000000000000001E-11</v>
+      </c>
+      <c r="M177">
+        <v>0</v>
+      </c>
+      <c r="N177">
+        <v>-1130</v>
+      </c>
+      <c r="O177">
+        <v>0</v>
+      </c>
+      <c r="P177">
+        <v>0</v>
+      </c>
+      <c r="Q177">
+        <v>0</v>
+      </c>
+      <c r="R177">
+        <v>0</v>
+      </c>
+      <c r="S177">
+        <v>0</v>
+      </c>
+      <c r="T177">
+        <v>0</v>
+      </c>
+      <c r="U177">
+        <v>0</v>
+      </c>
+      <c r="V177" t="s">
+        <v>522</v>
+      </c>
+      <c r="W177" t="s">
+        <v>523</v>
+      </c>
+      <c r="X177" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="Y177" t="s">
         <v>418</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed citation in model_setup
</commit_message>
<xml_diff>
--- a/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
+++ b/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01a63ffdd6170d0a/Desktop/copy REU Research/bluejay/Venus-Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5072E0A-A865-46C2-BD4F-868AE022A8D7}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA1BBDEB-939F-4C9D-A854-CB80CCB96AC5}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="900" windowWidth="21528" windowHeight="11832" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ion reactions" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9449" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9461" uniqueCount="546">
   <si>
     <t>R1</t>
   </si>
@@ -1666,6 +1666,9 @@
   <si>
     <t>This is not mass scaleing whitch I did use in the actual model</t>
   </si>
+  <si>
+    <t>Blitz, M.A.; McKee, K.W.; Pilling, M.J.  2000, NIST</t>
+  </si>
 </sst>
 </file>
 
@@ -46704,8 +46707,8 @@
   <dimension ref="A1:Y327"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F289" sqref="F289"/>
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B276" sqref="B276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -66711,7 +66714,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:E33"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -67834,11 +67837,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Y177"/>
+  <dimension ref="A1:Y180"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -73930,6 +73933,119 @@
         <v>479</v>
       </c>
       <c r="Y177" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="179" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B179" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D179" t="s">
+        <v>450</v>
+      </c>
+      <c r="E179" t="s">
+        <v>33</v>
+      </c>
+      <c r="G179">
+        <v>2</v>
+      </c>
+      <c r="L179" s="1">
+        <v>8.6E-11</v>
+      </c>
+      <c r="M179">
+        <v>0</v>
+      </c>
+      <c r="N179">
+        <v>0</v>
+      </c>
+      <c r="O179">
+        <v>0</v>
+      </c>
+      <c r="P179">
+        <v>0</v>
+      </c>
+      <c r="Q179">
+        <v>0</v>
+      </c>
+      <c r="R179">
+        <v>0</v>
+      </c>
+      <c r="S179">
+        <v>0</v>
+      </c>
+      <c r="T179">
+        <v>0</v>
+      </c>
+      <c r="U179">
+        <v>0</v>
+      </c>
+      <c r="V179">
+        <v>298</v>
+      </c>
+      <c r="W179" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y179" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C180" s="12"/>
+      <c r="D180" t="s">
+        <v>450</v>
+      </c>
+      <c r="E180" t="s">
+        <v>33</v>
+      </c>
+      <c r="G180">
+        <v>2</v>
+      </c>
+      <c r="L180" s="1">
+        <v>8.17E-11</v>
+      </c>
+      <c r="M180">
+        <v>0</v>
+      </c>
+      <c r="N180">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="O180">
+        <v>0</v>
+      </c>
+      <c r="P180">
+        <v>0</v>
+      </c>
+      <c r="Q180">
+        <v>0</v>
+      </c>
+      <c r="R180">
+        <v>0</v>
+      </c>
+      <c r="S180">
+        <v>0</v>
+      </c>
+      <c r="T180">
+        <v>0</v>
+      </c>
+      <c r="U180">
+        <v>0</v>
+      </c>
+      <c r="V180">
+        <v>298</v>
+      </c>
+      <c r="W180" t="s">
+        <v>545</v>
+      </c>
+      <c r="Y180" t="s">
         <v>418</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the mass scaling issues with some  dueterium species
</commit_message>
<xml_diff>
--- a/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
+++ b/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01a63ffdd6170d0a/Desktop/copy REU Research/bluejay/Venus-Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA1BBDEB-939F-4C9D-A854-CB80CCB96AC5}"/>
+  <xr:revisionPtr revIDLastSave="320" documentId="11_22B1562E36924AB92818D941A36D1037A47DC3BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E8C9A90-5080-46CB-80EF-697FBB841B2B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46707,8 +46707,8 @@
   <dimension ref="A1:Y327"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B276" sqref="B276"/>
+      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H298" sqref="H298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -63130,6 +63130,9 @@
       <c r="I288">
         <v>2</v>
       </c>
+      <c r="J288">
+        <v>-0.5</v>
+      </c>
       <c r="L288" s="1">
         <v>3.9000000000000001E-11</v>
       </c>
@@ -63193,6 +63196,9 @@
       <c r="I289">
         <v>2</v>
       </c>
+      <c r="J289">
+        <v>-0.5</v>
+      </c>
       <c r="L289" s="1">
         <v>3.9000000000000001E-11</v>
       </c>
@@ -63255,6 +63261,9 @@
       <c r="I290">
         <v>33</v>
       </c>
+      <c r="J290">
+        <v>-0.5</v>
+      </c>
       <c r="L290" s="1">
         <v>1.7999999999999999E-11</v>
       </c>
@@ -63317,6 +63326,9 @@
       <c r="I291">
         <v>2</v>
       </c>
+      <c r="J291">
+        <v>-0.5</v>
+      </c>
       <c r="L291" s="1">
         <v>9.9999999999999998E-13</v>
       </c>
@@ -63379,6 +63391,9 @@
       <c r="I292">
         <v>2</v>
       </c>
+      <c r="J292">
+        <v>-0.5</v>
+      </c>
       <c r="L292" s="1">
         <v>9.9999999999999998E-13</v>
       </c>
@@ -63441,6 +63456,9 @@
       <c r="I293">
         <v>17</v>
       </c>
+      <c r="J293">
+        <v>-0.5</v>
+      </c>
       <c r="L293" s="1">
         <v>1.7999999999999999E-11</v>
       </c>
@@ -63559,6 +63577,9 @@
       </c>
       <c r="I295">
         <v>1</v>
+      </c>
+      <c r="J295">
+        <v>-0.5</v>
       </c>
       <c r="L295" s="1">
         <v>1.4900000000000002E-11</v>

</xml_diff>

<commit_message>
fixed indentations, removed unessesary commented out lines, added some photolysis reaction sources that were missing, and fixed error regarding the H2Osatfrac that made it not work for Mars
</commit_message>
<xml_diff>
--- a/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
+++ b/Venus-Inputs/REACTION_NETWORK_VENUS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01a63ffdd6170d0a/Desktop/copy REU Research/bluejay/Venus-Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="455" documentId="13_ncr:1_{3E1F0C3F-1592-4064-8723-1B3B87D59E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0012F6F5-5151-4FCD-81BC-A90B732A0842}"/>
+  <xr:revisionPtr revIDLastSave="460" documentId="13_ncr:1_{3E1F0C3F-1592-4064-8723-1B3B87D59E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB600D30-46BF-4BDA-BE4A-B5C69173B63B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ion reactions" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,19 @@
     <sheet name="Unused ion reactions" sheetId="6" r:id="rId6"/>
     <sheet name="sulfur-chlorine planning" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -31,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10582" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10585" uniqueCount="694">
   <si>
     <t>R1</t>
   </si>
@@ -2105,6 +2116,15 @@
   <si>
     <t>Lizardo-Huerta, J.-C.; Sirjean, B.; Verdier, L.; Fournet, R.; Glaude, P.-A. 2018, NIST</t>
   </si>
+  <si>
+    <t>Hintze 2003 and Burkholder 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 2008,  Hintze 2003, Burkholder 2000, and Mills 2005 </t>
+  </si>
+  <si>
+    <t>Bahou 2001</t>
+  </si>
 </sst>
 </file>
 
@@ -2391,10 +2411,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2432,7 +2456,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2538,7 +2562,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2680,7 +2704,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -47296,7 +47320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA453"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A305" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R320" sqref="R320"/>
     </sheetView>
@@ -74281,9 +74305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -75467,6 +75491,9 @@
       <c r="K38" t="s">
         <v>44</v>
       </c>
+      <c r="U38" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -75548,6 +75575,9 @@
       <c r="K41" t="s">
         <v>44</v>
       </c>
+      <c r="U41" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -75614,6 +75644,9 @@
       </c>
       <c r="J43">
         <v>0</v>
+      </c>
+      <c r="U43" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>